<commit_message>
Unit model '3a - lca_it_pt' fixed and tested.
</commit_message>
<xml_diff>
--- a/tests/integration/models/3a - lca_it_pt/concept.xlsx
+++ b/tests/integration/models/3a - lca_it_pt/concept.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\models\3a - lca_it_pt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14780A3E-4A1A-49CF-85F9-DCC428A2009A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE6960D-3FE3-493E-8F17-8143F9CC8309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30870" yWindow="2680" windowWidth="28080" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hsut_hybrid assumptions" sheetId="8" r:id="rId1"/>
@@ -4879,10 +4879,10 @@
   <dimension ref="A1:AX43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="AD4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="AE4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R23" sqref="R23:AV25"/>
+      <selection pane="bottomRight" activeCell="AU19" sqref="AU19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6148,6 +6148,13 @@
       <c r="AF21" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="AR21" s="33"/>
+      <c r="AS21" s="33"/>
+      <c r="AT21" s="33"/>
+      <c r="AU21" s="33"/>
+      <c r="AV21" s="33"/>
+      <c r="AW21" s="33"/>
+      <c r="AX21" s="33"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.35">
       <c r="F22" s="3"/>
@@ -6167,15 +6174,43 @@
       <c r="AJ22" s="31">
         <v>5.078125</v>
       </c>
+      <c r="AR22" s="33"/>
+      <c r="AS22" s="33"/>
+      <c r="AT22" s="33"/>
+      <c r="AU22" s="33"/>
+      <c r="AV22" s="33"/>
+      <c r="AW22" s="33"/>
+      <c r="AX22" s="33"/>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.35">
       <c r="F23" s="3"/>
+      <c r="AR23" s="33"/>
+      <c r="AS23" s="33"/>
+      <c r="AT23" s="33"/>
+      <c r="AU23" s="33"/>
+      <c r="AV23" s="33"/>
+      <c r="AW23" s="33"/>
+      <c r="AX23" s="33"/>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.35">
       <c r="F24" s="3"/>
+      <c r="AR24" s="33"/>
+      <c r="AS24" s="33"/>
+      <c r="AT24" s="33"/>
+      <c r="AU24" s="33"/>
+      <c r="AV24" s="33"/>
+      <c r="AW24" s="33"/>
+      <c r="AX24" s="33"/>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.35">
       <c r="F25" s="3"/>
+      <c r="AR25" s="33"/>
+      <c r="AS25" s="33"/>
+      <c r="AT25" s="33"/>
+      <c r="AU25" s="33"/>
+      <c r="AV25" s="33"/>
+      <c r="AW25" s="33"/>
+      <c r="AX25" s="33"/>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.35">
       <c r="F26" s="3"/>

</xml_diff>

<commit_message>
Preparing case with two models for testing model linking. Adding the case to test cases.
</commit_message>
<xml_diff>
--- a/tests/integration/models/3a - lca_it_pt/concept.xlsx
+++ b/tests/integration/models/3a - lca_it_pt/concept.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\models\3a - lca_it_pt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE6960D-3FE3-493E-8F17-8143F9CC8309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBB6653-E40E-4F41-9D45-C889D4E05535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30870" yWindow="2680" windowWidth="28080" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hsut_hybrid assumptions" sheetId="8" r:id="rId1"/>
@@ -4878,11 +4878,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DB2726-940A-4A5E-B1C9-CC6BAC8BE2F9}">
   <dimension ref="A1:AX43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="AE4" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AU19" sqref="AU19"/>
+      <selection pane="bottomRight" activeCell="AL5" sqref="AL5:AM6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>